<commit_message>
Added models for search, suggestion, farewell and greetings Added intent Header to the database
</commit_message>
<xml_diff>
--- a/chatbot/database_intents.xlsx
+++ b/chatbot/database_intents.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DataScience\Machine Learning\Projects\Keepcoding\TFB\TFB-SmartBot\chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A22F3F7-46FA-4442-9D43-DA8DAC22160A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EC1505-081F-4D5A-B62E-C6E448350E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E701B219-9CB5-4FB1-A8B1-D6439049C12F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="127">
   <si>
     <t>Intent type</t>
   </si>
@@ -387,13 +387,37 @@
     <t>What can I do in this chatbot?</t>
   </si>
   <si>
-    <t>What options do I hace?</t>
-  </si>
-  <si>
     <t>Tell me what can I ask for</t>
   </si>
   <si>
     <t>Show me what you got</t>
+  </si>
+  <si>
+    <t>What options do I have?</t>
+  </si>
+  <si>
+    <t>How many options do I have?</t>
+  </si>
+  <si>
+    <t>Is there anything more I can do?</t>
+  </si>
+  <si>
+    <t>Headers</t>
+  </si>
+  <si>
+    <t>Tell me everything about Data Science</t>
+  </si>
+  <si>
+    <t>Show me more of Barcelona</t>
+  </si>
+  <si>
+    <t>What headers does this article have?</t>
+  </si>
+  <si>
+    <t>Give me more information please</t>
+  </si>
+  <si>
+    <t>I want to know more of Napoleon</t>
   </si>
 </sst>
 </file>
@@ -745,10 +769,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8947F2DF-9E18-4EF9-8E6E-53A318233C25}">
-  <dimension ref="A1:B114"/>
+  <dimension ref="A1:B121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1649,7 +1673,7 @@
         <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -1657,7 +1681,7 @@
         <v>114</v>
       </c>
       <c r="B113" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -1665,7 +1689,63 @@
         <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>118</v>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>114</v>
+      </c>
+      <c r="B115" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>114</v>
+      </c>
+      <c r="B116" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>121</v>
+      </c>
+      <c r="B117" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>121</v>
+      </c>
+      <c r="B118" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>121</v>
+      </c>
+      <c r="B119" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>121</v>
+      </c>
+      <c r="B120" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>121</v>
+      </c>
+      <c r="B121" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved models fixed error in chatbot that prevented long sentences to be predicted
</commit_message>
<xml_diff>
--- a/chatbot/database_intents.xlsx
+++ b/chatbot/database_intents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DataScience\Machine Learning\Projects\Keepcoding\TFB\TFB-SmartBot\chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EC1505-081F-4D5A-B62E-C6E448350E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1858BA-93A3-4C7E-B00D-3E851C9777FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E701B219-9CB5-4FB1-A8B1-D6439049C12F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="129">
   <si>
     <t>Intent type</t>
   </si>
@@ -418,6 +418,12 @@
   </si>
   <si>
     <t>I want to know more of Napoleon</t>
+  </si>
+  <si>
+    <t>Have a nice day</t>
+  </si>
+  <si>
+    <t>Bye</t>
   </si>
 </sst>
 </file>
@@ -769,10 +775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8947F2DF-9E18-4EF9-8E6E-53A318233C25}">
-  <dimension ref="A1:B121"/>
+  <dimension ref="A1:B123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B122" sqref="B122"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B113" sqref="B113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,18 +1668,18 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B111" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B112" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -1681,7 +1687,7 @@
         <v>114</v>
       </c>
       <c r="B113" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -1689,7 +1695,7 @@
         <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -1697,7 +1703,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -1705,23 +1711,23 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B117" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B118" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -1729,7 +1735,7 @@
         <v>121</v>
       </c>
       <c r="B119" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -1737,7 +1743,7 @@
         <v>121</v>
       </c>
       <c r="B120" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -1745,6 +1751,22 @@
         <v>121</v>
       </c>
       <c r="B121" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>121</v>
+      </c>
+      <c r="B123" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New model and improved Database
</commit_message>
<xml_diff>
--- a/chatbot/database_intents.xlsx
+++ b/chatbot/database_intents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DataScience\Machine Learning\Projects\Keepcoding\TFB\TFB-SmartBot\chatbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1858BA-93A3-4C7E-B00D-3E851C9777FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57134FA2-4579-42A0-BCD0-7EE46427FE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E701B219-9CB5-4FB1-A8B1-D6439049C12F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="114">
   <si>
     <t>Intent type</t>
   </si>
@@ -105,135 +105,9 @@
     <t>Search</t>
   </si>
   <si>
-    <t>I want to know more about Data Science</t>
-  </si>
-  <si>
-    <t>I want to search for John Lennon</t>
-  </si>
-  <si>
-    <t>Can you give information on the European Union?</t>
-  </si>
-  <si>
-    <t>Can you tell me about Data Science?</t>
-  </si>
-  <si>
-    <t>Give me information on aerodynamics</t>
-  </si>
-  <si>
-    <t>Tell me about Nina Simone</t>
-  </si>
-  <si>
-    <t>I want to know more about Steven Spilberg</t>
-  </si>
-  <si>
-    <t>Search for laplace rule</t>
-  </si>
-  <si>
-    <t>Look for quantum computing</t>
-  </si>
-  <si>
-    <t>I want info on Orion</t>
-  </si>
-  <si>
-    <t>Can you search for world war II</t>
-  </si>
-  <si>
-    <t>What can you tell me about The Godfather</t>
-  </si>
-  <si>
-    <t>Look in wikipedia for William Shakespeare</t>
-  </si>
-  <si>
-    <t>Search what wikipedia says about football</t>
-  </si>
-  <si>
-    <t>Search for nintendo</t>
-  </si>
-  <si>
-    <t>I want to search for gorilla</t>
-  </si>
-  <si>
-    <t>What is formula one?</t>
-  </si>
-  <si>
-    <t>What is ratatuille?</t>
-  </si>
-  <si>
-    <t>Give me info on Leonardo Dicaprio</t>
-  </si>
-  <si>
-    <t>Tell me about Andy Garcia</t>
-  </si>
-  <si>
     <t>Suggestions</t>
   </si>
   <si>
-    <t>Give me suggestions for animal</t>
-  </si>
-  <si>
-    <t>Tell me things related to cinema</t>
-  </si>
-  <si>
-    <t>What can you tell me related to electric guitar?</t>
-  </si>
-  <si>
-    <t>Give me suggestions for Mesopotamia</t>
-  </si>
-  <si>
-    <t>Tell me things related to aerospace engineering</t>
-  </si>
-  <si>
-    <t>Suggest me topics related to apple</t>
-  </si>
-  <si>
-    <t>Can you tell me about the roman empire?</t>
-  </si>
-  <si>
-    <t>I want to know things connected to New York</t>
-  </si>
-  <si>
-    <t>Tell me things connected to the spanish flu</t>
-  </si>
-  <si>
-    <t>Give suggestions for Frankenstein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suggest me something connected to the USSR </t>
-  </si>
-  <si>
-    <t>tell me things related to instagram</t>
-  </si>
-  <si>
-    <t>Can you name me things connected to bill gates?</t>
-  </si>
-  <si>
-    <t>What wikipedia says about data science?</t>
-  </si>
-  <si>
-    <t>What can you tell me connected to Gabriel García Marquez ?</t>
-  </si>
-  <si>
-    <t>I want to know what can you tell me that is linked to Paris</t>
-  </si>
-  <si>
-    <t>Can you suggest me concepts linked to artificial inteligence?</t>
-  </si>
-  <si>
-    <t>Tell me things connected to mercury</t>
-  </si>
-  <si>
-    <t>I want to know about things realated to gengis kan</t>
-  </si>
-  <si>
-    <t>Suggest me words related to Lolita</t>
-  </si>
-  <si>
-    <t>Give me suggestions for Nietzsche</t>
-  </si>
-  <si>
-    <t>Give me topics related to stand-up comedy</t>
-  </si>
-  <si>
     <t>Greeting</t>
   </si>
   <si>
@@ -270,81 +144,9 @@
     <t>It’s always a pleasure to see you.</t>
   </si>
   <si>
-    <t>Could you tell me about cryptocurrencies?</t>
-  </si>
-  <si>
-    <t>I wonder if you could explain what is socialism</t>
-  </si>
-  <si>
-    <t>I wonder if you could tell me information on Machine Learning</t>
-  </si>
-  <si>
-    <t>I wanna know everything about Psychology</t>
-  </si>
-  <si>
-    <t>I wanna know how a computer works</t>
-  </si>
-  <si>
-    <t>Please, search info about Johnny Depp</t>
-  </si>
-  <si>
     <t>I want to know more about it</t>
   </si>
   <si>
-    <t>What topics are related to Data Science?</t>
-  </si>
-  <si>
-    <t>I wanna know more about Bitcoin</t>
-  </si>
-  <si>
-    <t>Tell me things connected to aerospace engineering</t>
-  </si>
-  <si>
-    <t>Tell me things connected to cinema</t>
-  </si>
-  <si>
-    <t>What can you tell me connected to electric guitar?</t>
-  </si>
-  <si>
-    <t>Suggest me topics connected to apple</t>
-  </si>
-  <si>
-    <t>tell me things connected to instagram</t>
-  </si>
-  <si>
-    <t>Suggest me words connected to Lolita</t>
-  </si>
-  <si>
-    <t>Give me topics connected to stand-up comedy</t>
-  </si>
-  <si>
-    <t>What topics are connected to Data Science?</t>
-  </si>
-  <si>
-    <t>Tell me things linked to aerospace engineering</t>
-  </si>
-  <si>
-    <t>Tell me things linked to cinema</t>
-  </si>
-  <si>
-    <t>What can you tell me linked to electric guitar?</t>
-  </si>
-  <si>
-    <t>Suggest me topics linked to apple</t>
-  </si>
-  <si>
-    <t>tell me things linked to instagram</t>
-  </si>
-  <si>
-    <t>Suggest me words linked to Lolita</t>
-  </si>
-  <si>
-    <t>Give me topics linked to stand-up comedy</t>
-  </si>
-  <si>
-    <t>What topics are linked to Data Science?</t>
-  </si>
-  <si>
     <t>Farewell</t>
   </si>
   <si>
@@ -405,25 +207,178 @@
     <t>Headers</t>
   </si>
   <si>
-    <t>Tell me everything about Data Science</t>
-  </si>
-  <si>
-    <t>Show me more of Barcelona</t>
-  </si>
-  <si>
     <t>What headers does this article have?</t>
   </si>
   <si>
     <t>Give me more information please</t>
   </si>
   <si>
-    <t>I want to know more of Napoleon</t>
-  </si>
-  <si>
     <t>Have a nice day</t>
   </si>
   <si>
     <t>Bye</t>
+  </si>
+  <si>
+    <t>Give me info on entity</t>
+  </si>
+  <si>
+    <t>I want to know more about entity</t>
+  </si>
+  <si>
+    <t>I want to search for entity</t>
+  </si>
+  <si>
+    <t>Can you give information on the entity?</t>
+  </si>
+  <si>
+    <t>Can you tell me about the entity?</t>
+  </si>
+  <si>
+    <t>Give me information on entity</t>
+  </si>
+  <si>
+    <t>Tell me about entity</t>
+  </si>
+  <si>
+    <t>Search for entity</t>
+  </si>
+  <si>
+    <t>Look for entity</t>
+  </si>
+  <si>
+    <t>I want info on entity</t>
+  </si>
+  <si>
+    <t>Can you search for entity</t>
+  </si>
+  <si>
+    <t>What wikipedia says about entity?</t>
+  </si>
+  <si>
+    <t>Look in wikipedia for entity</t>
+  </si>
+  <si>
+    <t>Search what wikipedia says about entity</t>
+  </si>
+  <si>
+    <t>What can you tell me about entity</t>
+  </si>
+  <si>
+    <t>Can you tell me about entity?</t>
+  </si>
+  <si>
+    <t>What is entity?</t>
+  </si>
+  <si>
+    <t>Could you tell me about entity?</t>
+  </si>
+  <si>
+    <t>I wonder if you could tell me information on entity</t>
+  </si>
+  <si>
+    <t>I wonder if you could explain what is entity</t>
+  </si>
+  <si>
+    <t>I wanna know everything about entity</t>
+  </si>
+  <si>
+    <t>I wanna know how an entity works</t>
+  </si>
+  <si>
+    <t>Please, search info about entity</t>
+  </si>
+  <si>
+    <t>Tell me things related to entity</t>
+  </si>
+  <si>
+    <t>Give me suggestions for entity</t>
+  </si>
+  <si>
+    <t>What can you tell me related to entity?</t>
+  </si>
+  <si>
+    <t>Suggest me topics related to entity</t>
+  </si>
+  <si>
+    <t>I want to know things connected to entity</t>
+  </si>
+  <si>
+    <t>Tell me things connected to the entity</t>
+  </si>
+  <si>
+    <t>Give suggestions for entity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suggest me something connected to the entity </t>
+  </si>
+  <si>
+    <t>tell me things related to entity</t>
+  </si>
+  <si>
+    <t>Can you name me things connected to entity?</t>
+  </si>
+  <si>
+    <t>What can you tell me connected to entity?</t>
+  </si>
+  <si>
+    <t>I want to know what can you tell me that is linked to entity</t>
+  </si>
+  <si>
+    <t>Can you suggest me concepts linked to entity?</t>
+  </si>
+  <si>
+    <t>Tell me things connected to entity</t>
+  </si>
+  <si>
+    <t>I want to know about things realated to entity</t>
+  </si>
+  <si>
+    <t>Suggest me words related to entity</t>
+  </si>
+  <si>
+    <t>Give me topics related to entity</t>
+  </si>
+  <si>
+    <t>What topics are related to entity?</t>
+  </si>
+  <si>
+    <t>I wanna know more about entity</t>
+  </si>
+  <si>
+    <t>Suggest me topics connected to entity</t>
+  </si>
+  <si>
+    <t>tell me things connected to entity</t>
+  </si>
+  <si>
+    <t>Suggest me words connected to entity</t>
+  </si>
+  <si>
+    <t>Give me topics connected to entity</t>
+  </si>
+  <si>
+    <t>What topics are connected to entity?</t>
+  </si>
+  <si>
+    <t>Tell me things linked to entity</t>
+  </si>
+  <si>
+    <t>What can you tell me linked to entity?</t>
+  </si>
+  <si>
+    <t>Suggest me topics linked to entity</t>
+  </si>
+  <si>
+    <t>tell me things linked to entity</t>
+  </si>
+  <si>
+    <t>Suggest me words linked to entity</t>
+  </si>
+  <si>
+    <t>Give me topics linked to entity</t>
+  </si>
+  <si>
+    <t>What topics are linked to entity?</t>
   </si>
 </sst>
 </file>
@@ -775,11 +730,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8947F2DF-9E18-4EF9-8E6E-53A318233C25}">
-  <dimension ref="A1:B123"/>
+  <dimension ref="A1:B120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B113" sqref="B113"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -796,7 +749,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -804,7 +757,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -812,7 +765,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -820,7 +773,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -828,7 +781,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -836,7 +789,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -844,7 +797,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -852,7 +805,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -860,7 +813,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -868,7 +821,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -876,7 +829,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -884,7 +837,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
@@ -892,7 +845,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -900,7 +853,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -908,7 +861,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
@@ -916,7 +869,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -924,7 +877,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
@@ -932,7 +885,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
@@ -940,7 +893,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
@@ -948,90 +901,90 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1039,7 +992,7 @@
         <v>21</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1047,7 +1000,7 @@
         <v>21</v>
       </c>
       <c r="B33" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1055,7 +1008,7 @@
         <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1063,7 +1016,7 @@
         <v>21</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1071,7 +1024,7 @@
         <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1079,7 +1032,7 @@
         <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1087,7 +1040,7 @@
         <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1095,7 +1048,7 @@
         <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1103,7 +1056,7 @@
         <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1111,7 +1064,7 @@
         <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1119,7 +1072,7 @@
         <v>21</v>
       </c>
       <c r="B42" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1127,7 +1080,7 @@
         <v>21</v>
       </c>
       <c r="B43" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -1135,7 +1088,7 @@
         <v>21</v>
       </c>
       <c r="B44" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1143,7 +1096,7 @@
         <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1151,7 +1104,7 @@
         <v>21</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -1159,7 +1112,7 @@
         <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1167,7 +1120,7 @@
         <v>21</v>
       </c>
       <c r="B48" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -1175,7 +1128,7 @@
         <v>21</v>
       </c>
       <c r="B49" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -1183,7 +1136,7 @@
         <v>21</v>
       </c>
       <c r="B50" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1191,7 +1144,7 @@
         <v>21</v>
       </c>
       <c r="B51" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1199,7 +1152,7 @@
         <v>21</v>
       </c>
       <c r="B52" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1207,7 +1160,7 @@
         <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1215,7 +1168,7 @@
         <v>21</v>
       </c>
       <c r="B54" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1231,7 +1184,7 @@
         <v>21</v>
       </c>
       <c r="B56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1239,7 +1192,7 @@
         <v>21</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1268,506 +1221,482 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B61" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B62" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B63" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B64" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B65" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B66" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B67" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B68" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B69" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B70" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B71" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B72" t="s">
-        <v>55</v>
+        <v>92</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B73" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B74" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B75" t="s">
-        <v>59</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B76" t="s">
-        <v>60</v>
+        <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B77" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B78" t="s">
-        <v>62</v>
+        <v>98</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B79" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B80" t="s">
-        <v>64</v>
+        <v>99</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B81" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B82" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B83" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B84" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B85" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B86" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B87" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B88" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B89" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B90" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B91" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B92" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B93" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B94" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B95" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B96" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B97" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B98" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B99" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="B100" t="s">
-        <v>103</v>
+        <v>37</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="B101" t="s">
-        <v>104</v>
+        <v>38</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="B102" t="s">
-        <v>105</v>
+        <v>39</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="B103" t="s">
-        <v>106</v>
+        <v>40</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="B104" t="s">
-        <v>107</v>
+        <v>41</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="B105" t="s">
-        <v>108</v>
+        <v>42</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="B106" t="s">
-        <v>109</v>
+        <v>43</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="B107" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="B108" t="s">
-        <v>111</v>
+        <v>45</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="B109" t="s">
-        <v>112</v>
+        <v>46</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="B110" t="s">
-        <v>113</v>
+        <v>47</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="B111" t="s">
-        <v>127</v>
+        <v>58</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>102</v>
+        <v>36</v>
       </c>
       <c r="B112" t="s">
-        <v>128</v>
+        <v>59</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>114</v>
+        <v>48</v>
       </c>
       <c r="B113" t="s">
-        <v>115</v>
+        <v>49</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>114</v>
+        <v>48</v>
       </c>
       <c r="B114" t="s">
-        <v>118</v>
+        <v>52</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>114</v>
+        <v>48</v>
       </c>
       <c r="B115" t="s">
-        <v>116</v>
+        <v>50</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>114</v>
+        <v>48</v>
       </c>
       <c r="B116" t="s">
-        <v>117</v>
+        <v>51</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>114</v>
+        <v>48</v>
       </c>
       <c r="B117" t="s">
-        <v>119</v>
+        <v>53</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>114</v>
+        <v>48</v>
       </c>
       <c r="B118" t="s">
-        <v>120</v>
+        <v>54</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>121</v>
+        <v>55</v>
       </c>
       <c r="B119" t="s">
-        <v>122</v>
+        <v>56</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>121</v>
+        <v>55</v>
       </c>
       <c r="B120" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>121</v>
-      </c>
-      <c r="B121" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>121</v>
-      </c>
-      <c r="B122" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>121</v>
-      </c>
-      <c r="B123" t="s">
-        <v>126</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>